<commit_message>
matched province fully for PubObsStationX
</commit_message>
<xml_diff>
--- a/data-raw/data-tidy/public-site/observe-station/xlsx/list-most-2021.xlsx
+++ b/data-raw/data-tidy/public-site/observe-station/xlsx/list-most-2021.xlsx
@@ -230,6 +230,9 @@
     <t xml:space="preserve">国家海洋局南海环境监测中心、自然资源部第三海洋研究所</t>
   </si>
   <si>
+    <t xml:space="preserve">广东</t>
+  </si>
+  <si>
     <t xml:space="preserve">13</t>
   </si>
   <si>
@@ -269,9 +272,6 @@
     <t xml:space="preserve">生态环境部</t>
   </si>
   <si>
-    <t xml:space="preserve">广东</t>
-  </si>
-  <si>
     <t xml:space="preserve">17</t>
   </si>
   <si>
@@ -293,550 +293,550 @@
     <t xml:space="preserve">中交第一公路勘察设计研究院有限公司、青海省交通科学研究院</t>
   </si>
   <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">广东港珠澳大桥材料腐蚀与工程安全国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">港珠澳大桥管理局</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">内蒙古阴山北麓草原生态水文国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国水利水电科学研究院</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水利部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山西寿阳旱地农业生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国农业科学院农业环境与可持续发展研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">农业农村部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">云南大理农业生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">农业农村部环境保护科研监测所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">天津</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">海南儋州热带农业生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国热带农业科学院</t>
+  </si>
+  <si>
+    <t xml:space="preserve">海南</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山东长岛近海渔业资源国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国水产科学研究院黄海水产研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山东</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">江苏南京水稻种质资源国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">南京农业大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">农业农村部、教育部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">云南昆明电磁波环境国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国电子科技集团公司第二十二研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">国资委</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河南</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河南宝天曼森林生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国林业科学研究院森林生态环境与保护研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">林草局</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河南黄河小浪底地球关键带国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国林业科学研究院林业研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陕西秦岭大熊猫金丝猴生物多样性国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院动物研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中科院</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浙江钱江源森林生物多样性国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院植物研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">黑龙江兴凯湖湖泊湿地生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院东北地理与农业生态研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中科院、黑龙江省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">辽宁清原森林生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院沈阳应用生态研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">辽宁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">江西千烟洲红壤丘陵地球关键带国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院地理科学与资源研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北京燕山地球关键带国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">海南西沙海洋环境国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院南海海洋研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西藏纳木错高寒湖泊与环境国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院青藏高原研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">云南丽江玉龙雪山冰冻圈与可持续发展国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院西北生态环境资源研究院</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西藏珠穆朗玛特殊大气过程与环境变化国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北京京津冀区域生态环境变化与综合治理国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院生态环境研究中心</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">黑龙江漠河地球物理国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院地质与地球物理研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">青海北麓河高原冻土工程安全国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新疆帕米尔陆内俯冲国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国地震局地质研究所、新疆维吾尔自治区地震局</t>
+  </si>
+  <si>
+    <t xml:space="preserve">地震局</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河北红山巨厚沉积与地震灾害国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河北省地震局、北京大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河北</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新疆塔克拉玛干沙漠气象国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国气象局乌鲁木齐沙漠气象研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">气象局</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新疆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河北固城农业气象国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国气象科学研究院</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">天津环渤海滨海地球关键带国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">天津大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">天津市科学技术局</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河北塞罕坝人工林生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北京大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河北省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">辽宁盘锦湿地生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">沈阳农业大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">辽宁省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吉林大安农田生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吉林省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">上海长三角城市湿地生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">上海师范大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">上海市科学技术委员会</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">上海长江河口湿地生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">复旦大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">福建三明森林生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">福建师范大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">福建省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">江西鄱阳湖湖泊湿地生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院南京地理与湖泊研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">江西省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河南大别山森林生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河南大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河南省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">湖南洞庭湖湖泊湿地生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院亚热带农业生态研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">湖南省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">湖南</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">广东南岭森林生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">广东省科学院广州地理研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">广东省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">重庆金佛山喀斯特生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西南大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">重庆市科学技术局</t>
+  </si>
+  <si>
+    <t xml:space="preserve">重庆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">湖南雪峰山能源装备安全国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">重庆大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">四川若尔盖高寒湿地生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西南民族大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">四川省科学技术厅、国家民委</t>
+  </si>
+  <si>
+    <t xml:space="preserve">四川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">贵州普定喀斯特生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院地球化学研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">贵州省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">贵州</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">云南洱海湖泊生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">上海交通大学、上海交通大学云南（大理）研究院</t>
+  </si>
+  <si>
+    <t xml:space="preserve">云南省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">云南丽江森林生物多样性国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院昆明植物研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">云南</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西藏那曲高寒草地生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院地理科学与资源研究所、中国科学院青藏高原研究所、西藏大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西藏自治区科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西藏羊八井高海拔电气安全与电磁环境国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国电力科学研究院有限公司、国网西藏电力有限公司</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陕西黄土高原地球关键带国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院地球环境研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陕西省科学技术厅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陕西关中平原区域生态环境变化与综合治理国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">青海三江源草地生态系统国家野外科学观测研究站</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中国科学院西北高原生物研究所、青海大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">青海省科学技术厅</t>
+  </si>
+  <si>
     <t xml:space="preserve">青海</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">广东港珠澳大桥材料腐蚀与工程安全国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">港珠澳大桥管理局</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">内蒙古阴山北麓草原生态水文国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国水利水电科学研究院</t>
-  </si>
-  <si>
-    <t xml:space="preserve">水利部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">山西寿阳旱地农业生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国农业科学院农业环境与可持续发展研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">农业农村部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">云南大理农业生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">农业农村部环境保护科研监测所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">天津</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">海南儋州热带农业生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国热带农业科学院</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">山东长岛近海渔业资源国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国水产科学研究院黄海水产研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">山东</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">江苏南京水稻种质资源国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">南京农业大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">农业农村部、教育部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">云南昆明电磁波环境国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国电子科技集团公司第二十二研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">国资委</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河南宝天曼森林生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国林业科学研究院森林生态环境与保护研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">林草局</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河南黄河小浪底地球关键带国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国林业科学研究院林业研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">陕西秦岭大熊猫金丝猴生物多样性国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院动物研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中科院</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">浙江钱江源森林生物多样性国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院植物研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">黑龙江兴凯湖湖泊湿地生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院东北地理与农业生态研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中科院、黑龙江省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">辽宁清原森林生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院沈阳应用生态研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">辽宁</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">江西千烟洲红壤丘陵地球关键带国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院地理科学与资源研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">北京燕山地球关键带国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">海南西沙海洋环境国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院南海海洋研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">西藏纳木错高寒湖泊与环境国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院青藏高原研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">云南丽江玉龙雪山冰冻圈与可持续发展国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院西北生态环境资源研究院</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">西藏珠穆朗玛特殊大气过程与环境变化国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">北京京津冀区域生态环境变化与综合治理国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院生态环境研究中心</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">黑龙江漠河地球物理国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院地质与地球物理研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">青海北麓河高原冻土工程安全国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">新疆帕米尔陆内俯冲国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国地震局地质研究所、新疆维吾尔自治区地震局</t>
-  </si>
-  <si>
-    <t xml:space="preserve">地震局</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河北红山巨厚沉积与地震灾害国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河北省地震局、北京大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河北</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">新疆塔克拉玛干沙漠气象国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国气象局乌鲁木齐沙漠气象研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">气象局</t>
-  </si>
-  <si>
-    <t xml:space="preserve">新疆</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河北固城农业气象国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国气象科学研究院</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">天津环渤海滨海地球关键带国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">天津大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">天津市科学技术局</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河北塞罕坝人工林生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">北京大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河北省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">辽宁盘锦湿地生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">沈阳农业大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">辽宁省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">吉林大安农田生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">吉林省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">上海长三角城市湿地生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">上海师范大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">上海市科学技术委员会</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">上海长江河口湿地生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">复旦大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">福建三明森林生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">福建师范大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">福建省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">江西鄱阳湖湖泊湿地生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院南京地理与湖泊研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">江西省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河南大别山森林生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河南大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河南省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">河南</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">湖南洞庭湖湖泊湿地生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院亚热带农业生态研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">湖南省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">湖南</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">广东南岭森林生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">广东省科学院广州地理研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">广东省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">重庆金佛山喀斯特生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">西南大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">重庆市科学技术局</t>
-  </si>
-  <si>
-    <t xml:space="preserve">重庆</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">湖南雪峰山能源装备安全国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">重庆大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">四川若尔盖高寒湿地生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">西南民族大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">四川省科学技术厅、国家民委</t>
-  </si>
-  <si>
-    <t xml:space="preserve">四川</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">贵州普定喀斯特生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院地球化学研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">贵州省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">贵州</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">云南洱海湖泊生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">上海交通大学、上海交通大学云南（大理）研究院</t>
-  </si>
-  <si>
-    <t xml:space="preserve">云南省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">云南丽江森林生物多样性国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院昆明植物研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">云南</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">西藏那曲高寒草地生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院地理科学与资源研究所、中国科学院青藏高原研究所、西藏大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">西藏自治区科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">西藏羊八井高海拔电气安全与电磁环境国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国电力科学研究院有限公司、国网西藏电力有限公司</t>
-  </si>
-  <si>
-    <t xml:space="preserve">西藏</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">陕西黄土高原地球关键带国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院地球环境研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">陕西省科学技术厅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">陕西关中平原区域生态环境变化与综合治理国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">青海三江源草地生态系统国家野外科学观测研究站</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中国科学院西北高原生物研究所、青海大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">青海省科学技术厅</t>
   </si>
   <si>
     <t xml:space="preserve">68</t>
@@ -2606,7 +2606,9 @@
       <c r="G49" t="s">
         <v>26</v>
       </c>
-      <c r="H49"/>
+      <c r="H49" t="s">
+        <v>72</v>
+      </c>
       <c r="I49" t="s">
         <v>28</v>
       </c>
@@ -2622,7 +2624,7 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -2634,7 +2636,7 @@
         <v>14</v>
       </c>
       <c r="H50" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I50" t="s">
         <v>16</v>
@@ -2651,7 +2653,7 @@
         <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -2663,7 +2665,7 @@
         <v>18</v>
       </c>
       <c r="H51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I51" t="s">
         <v>20</v>
@@ -2680,7 +2682,7 @@
         <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -2709,7 +2711,7 @@
         <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -2720,7 +2722,9 @@
       <c r="G53" t="s">
         <v>26</v>
       </c>
-      <c r="H53"/>
+      <c r="H53" t="s">
+        <v>47</v>
+      </c>
       <c r="I53" t="s">
         <v>28</v>
       </c>
@@ -2736,7 +2740,7 @@
         <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E54" t="s">
         <v>12</v>
@@ -2748,7 +2752,7 @@
         <v>14</v>
       </c>
       <c r="H54" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I54" t="s">
         <v>16</v>
@@ -2765,7 +2769,7 @@
         <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -2777,7 +2781,7 @@
         <v>18</v>
       </c>
       <c r="H55" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I55" t="s">
         <v>20</v>
@@ -2794,7 +2798,7 @@
         <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -2823,7 +2827,7 @@
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -2852,7 +2856,7 @@
         <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E58" t="s">
         <v>12</v>
@@ -2864,7 +2868,7 @@
         <v>14</v>
       </c>
       <c r="H58" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I58" t="s">
         <v>16</v>
@@ -2881,7 +2885,7 @@
         <v>10</v>
       </c>
       <c r="D59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E59" t="s">
         <v>12</v>
@@ -2893,7 +2897,7 @@
         <v>18</v>
       </c>
       <c r="H59" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I59" t="s">
         <v>20</v>
@@ -2910,7 +2914,7 @@
         <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E60" t="s">
         <v>12</v>
@@ -2939,7 +2943,7 @@
         <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E61" t="s">
         <v>12</v>
@@ -2968,7 +2972,7 @@
         <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E62" t="s">
         <v>12</v>
@@ -2980,7 +2984,7 @@
         <v>14</v>
       </c>
       <c r="H62" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I62" t="s">
         <v>16</v>
@@ -2997,7 +3001,7 @@
         <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E63" t="s">
         <v>12</v>
@@ -3009,7 +3013,7 @@
         <v>18</v>
       </c>
       <c r="H63" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I63" t="s">
         <v>20</v>
@@ -3026,7 +3030,7 @@
         <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E64" t="s">
         <v>12</v>
@@ -3038,7 +3042,7 @@
         <v>22</v>
       </c>
       <c r="H64" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I64" t="s">
         <v>24</v>
@@ -3055,7 +3059,7 @@
         <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E65" t="s">
         <v>12</v>
@@ -3067,7 +3071,7 @@
         <v>26</v>
       </c>
       <c r="H65" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="I65" t="s">
         <v>28</v>
@@ -3299,7 +3303,7 @@
         <v>26</v>
       </c>
       <c r="H73" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="I73" t="s">
         <v>28</v>
@@ -3316,7 +3320,7 @@
         <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E74" t="s">
         <v>12</v>
@@ -3328,7 +3332,7 @@
         <v>14</v>
       </c>
       <c r="H74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I74" t="s">
         <v>16</v>
@@ -3345,7 +3349,7 @@
         <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E75" t="s">
         <v>12</v>
@@ -3357,7 +3361,7 @@
         <v>18</v>
       </c>
       <c r="H75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I75" t="s">
         <v>20</v>
@@ -3374,7 +3378,7 @@
         <v>10</v>
       </c>
       <c r="D76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E76" t="s">
         <v>12</v>
@@ -3403,7 +3407,7 @@
         <v>10</v>
       </c>
       <c r="D77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E77" t="s">
         <v>12</v>
@@ -3414,7 +3418,9 @@
       <c r="G77" t="s">
         <v>26</v>
       </c>
-      <c r="H77"/>
+      <c r="H77" t="s">
+        <v>72</v>
+      </c>
       <c r="I77" t="s">
         <v>28</v>
       </c>
@@ -3430,7 +3436,7 @@
         <v>10</v>
       </c>
       <c r="D78" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E78" t="s">
         <v>12</v>
@@ -3442,7 +3448,7 @@
         <v>14</v>
       </c>
       <c r="H78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I78" t="s">
         <v>16</v>
@@ -3459,7 +3465,7 @@
         <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E79" t="s">
         <v>12</v>
@@ -3471,7 +3477,7 @@
         <v>18</v>
       </c>
       <c r="H79" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I79" t="s">
         <v>20</v>
@@ -3488,7 +3494,7 @@
         <v>10</v>
       </c>
       <c r="D80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E80" t="s">
         <v>12</v>
@@ -3500,7 +3506,7 @@
         <v>22</v>
       </c>
       <c r="H80" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I80" t="s">
         <v>24</v>
@@ -3517,7 +3523,7 @@
         <v>10</v>
       </c>
       <c r="D81" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E81" t="s">
         <v>12</v>
@@ -3546,7 +3552,7 @@
         <v>10</v>
       </c>
       <c r="D82" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E82" t="s">
         <v>12</v>
@@ -3558,7 +3564,7 @@
         <v>14</v>
       </c>
       <c r="H82" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I82" t="s">
         <v>16</v>
@@ -3575,7 +3581,7 @@
         <v>10</v>
       </c>
       <c r="D83" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E83" t="s">
         <v>12</v>
@@ -3587,7 +3593,7 @@
         <v>18</v>
       </c>
       <c r="H83" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I83" t="s">
         <v>20</v>
@@ -3604,7 +3610,7 @@
         <v>10</v>
       </c>
       <c r="D84" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E84" t="s">
         <v>12</v>
@@ -3616,7 +3622,7 @@
         <v>22</v>
       </c>
       <c r="H84" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I84" t="s">
         <v>24</v>
@@ -3633,7 +3639,7 @@
         <v>10</v>
       </c>
       <c r="D85" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E85" t="s">
         <v>12</v>
@@ -3662,7 +3668,7 @@
         <v>10</v>
       </c>
       <c r="D86" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E86" t="s">
         <v>12</v>
@@ -3674,7 +3680,7 @@
         <v>14</v>
       </c>
       <c r="H86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I86" t="s">
         <v>16</v>
@@ -3691,7 +3697,7 @@
         <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E87" t="s">
         <v>12</v>
@@ -3703,7 +3709,7 @@
         <v>18</v>
       </c>
       <c r="H87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I87" t="s">
         <v>20</v>
@@ -3720,7 +3726,7 @@
         <v>10</v>
       </c>
       <c r="D88" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E88" t="s">
         <v>12</v>
@@ -3732,7 +3738,7 @@
         <v>22</v>
       </c>
       <c r="H88" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I88" t="s">
         <v>24</v>
@@ -3749,7 +3755,7 @@
         <v>10</v>
       </c>
       <c r="D89" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E89" t="s">
         <v>12</v>
@@ -3761,7 +3767,7 @@
         <v>26</v>
       </c>
       <c r="H89" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I89" t="s">
         <v>28</v>
@@ -3778,7 +3784,7 @@
         <v>10</v>
       </c>
       <c r="D90" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E90" t="s">
         <v>12</v>
@@ -3790,7 +3796,7 @@
         <v>14</v>
       </c>
       <c r="H90" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I90" t="s">
         <v>16</v>
@@ -3807,7 +3813,7 @@
         <v>10</v>
       </c>
       <c r="D91" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E91" t="s">
         <v>12</v>
@@ -3819,7 +3825,7 @@
         <v>18</v>
       </c>
       <c r="H91" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I91" t="s">
         <v>20</v>
@@ -3836,7 +3842,7 @@
         <v>10</v>
       </c>
       <c r="D92" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E92" t="s">
         <v>12</v>
@@ -3848,7 +3854,7 @@
         <v>22</v>
       </c>
       <c r="H92" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I92" t="s">
         <v>24</v>
@@ -3865,7 +3871,7 @@
         <v>10</v>
       </c>
       <c r="D93" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E93" t="s">
         <v>12</v>
@@ -3876,7 +3882,9 @@
       <c r="G93" t="s">
         <v>26</v>
       </c>
-      <c r="H93"/>
+      <c r="H93" t="s">
+        <v>111</v>
+      </c>
       <c r="I93" t="s">
         <v>28</v>
       </c>
@@ -3962,7 +3970,7 @@
         <v>22</v>
       </c>
       <c r="H96" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I96" t="s">
         <v>24</v>
@@ -4222,7 +4230,9 @@
       <c r="G105" t="s">
         <v>26</v>
       </c>
-      <c r="H105"/>
+      <c r="H105" t="s">
+        <v>124</v>
+      </c>
       <c r="I105" t="s">
         <v>28</v>
       </c>
@@ -4238,7 +4248,7 @@
         <v>10</v>
       </c>
       <c r="D106" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E106" t="s">
         <v>12</v>
@@ -4250,7 +4260,7 @@
         <v>14</v>
       </c>
       <c r="H106" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I106" t="s">
         <v>16</v>
@@ -4267,7 +4277,7 @@
         <v>10</v>
       </c>
       <c r="D107" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E107" t="s">
         <v>12</v>
@@ -4279,7 +4289,7 @@
         <v>18</v>
       </c>
       <c r="H107" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I107" t="s">
         <v>20</v>
@@ -4296,7 +4306,7 @@
         <v>10</v>
       </c>
       <c r="D108" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E108" t="s">
         <v>12</v>
@@ -4308,7 +4318,7 @@
         <v>22</v>
       </c>
       <c r="H108" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I108" t="s">
         <v>24</v>
@@ -4325,7 +4335,7 @@
         <v>10</v>
       </c>
       <c r="D109" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E109" t="s">
         <v>12</v>
@@ -4354,7 +4364,7 @@
         <v>10</v>
       </c>
       <c r="D110" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E110" t="s">
         <v>12</v>
@@ -4366,7 +4376,7 @@
         <v>14</v>
       </c>
       <c r="H110" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I110" t="s">
         <v>16</v>
@@ -4383,7 +4393,7 @@
         <v>10</v>
       </c>
       <c r="D111" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E111" t="s">
         <v>12</v>
@@ -4395,7 +4405,7 @@
         <v>18</v>
       </c>
       <c r="H111" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I111" t="s">
         <v>20</v>
@@ -4412,7 +4422,7 @@
         <v>10</v>
       </c>
       <c r="D112" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E112" t="s">
         <v>12</v>
@@ -4424,7 +4434,7 @@
         <v>22</v>
       </c>
       <c r="H112" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I112" t="s">
         <v>24</v>
@@ -4441,7 +4451,7 @@
         <v>10</v>
       </c>
       <c r="D113" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E113" t="s">
         <v>12</v>
@@ -4470,7 +4480,7 @@
         <v>10</v>
       </c>
       <c r="D114" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E114" t="s">
         <v>12</v>
@@ -4482,7 +4492,7 @@
         <v>14</v>
       </c>
       <c r="H114" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I114" t="s">
         <v>16</v>
@@ -4499,7 +4509,7 @@
         <v>10</v>
       </c>
       <c r="D115" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E115" t="s">
         <v>12</v>
@@ -4511,7 +4521,7 @@
         <v>18</v>
       </c>
       <c r="H115" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I115" t="s">
         <v>20</v>
@@ -4528,7 +4538,7 @@
         <v>10</v>
       </c>
       <c r="D116" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E116" t="s">
         <v>12</v>
@@ -4540,7 +4550,7 @@
         <v>22</v>
       </c>
       <c r="H116" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I116" t="s">
         <v>24</v>
@@ -4557,7 +4567,7 @@
         <v>10</v>
       </c>
       <c r="D117" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E117" t="s">
         <v>12</v>
@@ -4586,7 +4596,7 @@
         <v>10</v>
       </c>
       <c r="D118" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E118" t="s">
         <v>12</v>
@@ -4598,7 +4608,7 @@
         <v>14</v>
       </c>
       <c r="H118" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I118" t="s">
         <v>16</v>
@@ -4615,7 +4625,7 @@
         <v>10</v>
       </c>
       <c r="D119" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E119" t="s">
         <v>12</v>
@@ -4627,7 +4637,7 @@
         <v>18</v>
       </c>
       <c r="H119" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I119" t="s">
         <v>20</v>
@@ -4644,7 +4654,7 @@
         <v>10</v>
       </c>
       <c r="D120" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E120" t="s">
         <v>12</v>
@@ -4656,7 +4666,7 @@
         <v>22</v>
       </c>
       <c r="H120" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I120" t="s">
         <v>24</v>
@@ -4673,7 +4683,7 @@
         <v>10</v>
       </c>
       <c r="D121" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E121" t="s">
         <v>12</v>
@@ -4702,7 +4712,7 @@
         <v>10</v>
       </c>
       <c r="D122" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E122" t="s">
         <v>12</v>
@@ -4714,7 +4724,7 @@
         <v>14</v>
       </c>
       <c r="H122" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I122" t="s">
         <v>16</v>
@@ -4731,7 +4741,7 @@
         <v>10</v>
       </c>
       <c r="D123" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E123" t="s">
         <v>12</v>
@@ -4743,7 +4753,7 @@
         <v>18</v>
       </c>
       <c r="H123" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I123" t="s">
         <v>20</v>
@@ -4760,7 +4770,7 @@
         <v>10</v>
       </c>
       <c r="D124" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E124" t="s">
         <v>12</v>
@@ -4772,7 +4782,7 @@
         <v>22</v>
       </c>
       <c r="H124" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I124" t="s">
         <v>24</v>
@@ -4789,7 +4799,7 @@
         <v>10</v>
       </c>
       <c r="D125" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E125" t="s">
         <v>12</v>
@@ -4818,7 +4828,7 @@
         <v>10</v>
       </c>
       <c r="D126" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E126" t="s">
         <v>12</v>
@@ -4830,7 +4840,7 @@
         <v>14</v>
       </c>
       <c r="H126" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I126" t="s">
         <v>16</v>
@@ -4847,7 +4857,7 @@
         <v>10</v>
       </c>
       <c r="D127" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E127" t="s">
         <v>12</v>
@@ -4859,7 +4869,7 @@
         <v>18</v>
       </c>
       <c r="H127" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I127" t="s">
         <v>20</v>
@@ -4876,7 +4886,7 @@
         <v>10</v>
       </c>
       <c r="D128" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E128" t="s">
         <v>12</v>
@@ -4888,7 +4898,7 @@
         <v>22</v>
       </c>
       <c r="H128" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I128" t="s">
         <v>24</v>
@@ -4905,7 +4915,7 @@
         <v>10</v>
       </c>
       <c r="D129" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E129" t="s">
         <v>12</v>
@@ -4917,7 +4927,7 @@
         <v>26</v>
       </c>
       <c r="H129" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I129" t="s">
         <v>28</v>
@@ -4934,7 +4944,7 @@
         <v>10</v>
       </c>
       <c r="D130" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E130" t="s">
         <v>12</v>
@@ -4946,7 +4956,7 @@
         <v>14</v>
       </c>
       <c r="H130" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I130" t="s">
         <v>16</v>
@@ -4963,7 +4973,7 @@
         <v>10</v>
       </c>
       <c r="D131" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E131" t="s">
         <v>12</v>
@@ -4975,7 +4985,7 @@
         <v>18</v>
       </c>
       <c r="H131" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I131" t="s">
         <v>20</v>
@@ -4992,7 +5002,7 @@
         <v>10</v>
       </c>
       <c r="D132" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E132" t="s">
         <v>12</v>
@@ -5004,7 +5014,7 @@
         <v>22</v>
       </c>
       <c r="H132" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I132" t="s">
         <v>24</v>
@@ -5021,7 +5031,7 @@
         <v>10</v>
       </c>
       <c r="D133" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E133" t="s">
         <v>12</v>
@@ -5050,7 +5060,7 @@
         <v>10</v>
       </c>
       <c r="D134" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E134" t="s">
         <v>12</v>
@@ -5062,7 +5072,7 @@
         <v>14</v>
       </c>
       <c r="H134" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I134" t="s">
         <v>16</v>
@@ -5079,7 +5089,7 @@
         <v>10</v>
       </c>
       <c r="D135" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E135" t="s">
         <v>12</v>
@@ -5091,7 +5101,7 @@
         <v>18</v>
       </c>
       <c r="H135" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I135" t="s">
         <v>20</v>
@@ -5108,7 +5118,7 @@
         <v>10</v>
       </c>
       <c r="D136" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E136" t="s">
         <v>12</v>
@@ -5120,7 +5130,7 @@
         <v>22</v>
       </c>
       <c r="H136" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I136" t="s">
         <v>24</v>
@@ -5137,7 +5147,7 @@
         <v>10</v>
       </c>
       <c r="D137" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E137" t="s">
         <v>12</v>
@@ -5166,7 +5176,7 @@
         <v>10</v>
       </c>
       <c r="D138" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E138" t="s">
         <v>12</v>
@@ -5178,7 +5188,7 @@
         <v>14</v>
       </c>
       <c r="H138" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I138" t="s">
         <v>16</v>
@@ -5195,7 +5205,7 @@
         <v>10</v>
       </c>
       <c r="D139" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E139" t="s">
         <v>12</v>
@@ -5207,7 +5217,7 @@
         <v>18</v>
       </c>
       <c r="H139" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I139" t="s">
         <v>20</v>
@@ -5224,7 +5234,7 @@
         <v>10</v>
       </c>
       <c r="D140" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E140" t="s">
         <v>12</v>
@@ -5236,7 +5246,7 @@
         <v>22</v>
       </c>
       <c r="H140" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I140" t="s">
         <v>24</v>
@@ -5253,7 +5263,7 @@
         <v>10</v>
       </c>
       <c r="D141" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E141" t="s">
         <v>12</v>
@@ -5265,7 +5275,7 @@
         <v>26</v>
       </c>
       <c r="H141" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="I141" t="s">
         <v>28</v>
@@ -5282,7 +5292,7 @@
         <v>10</v>
       </c>
       <c r="D142" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E142" t="s">
         <v>12</v>
@@ -5294,7 +5304,7 @@
         <v>14</v>
       </c>
       <c r="H142" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I142" t="s">
         <v>16</v>
@@ -5311,7 +5321,7 @@
         <v>10</v>
       </c>
       <c r="D143" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E143" t="s">
         <v>12</v>
@@ -5323,7 +5333,7 @@
         <v>18</v>
       </c>
       <c r="H143" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I143" t="s">
         <v>20</v>
@@ -5340,7 +5350,7 @@
         <v>10</v>
       </c>
       <c r="D144" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E144" t="s">
         <v>12</v>
@@ -5352,7 +5362,7 @@
         <v>22</v>
       </c>
       <c r="H144" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I144" t="s">
         <v>24</v>
@@ -5369,7 +5379,7 @@
         <v>10</v>
       </c>
       <c r="D145" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E145" t="s">
         <v>12</v>
@@ -5398,7 +5408,7 @@
         <v>10</v>
       </c>
       <c r="D146" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E146" t="s">
         <v>12</v>
@@ -5410,7 +5420,7 @@
         <v>14</v>
       </c>
       <c r="H146" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I146" t="s">
         <v>16</v>
@@ -5427,7 +5437,7 @@
         <v>10</v>
       </c>
       <c r="D147" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E147" t="s">
         <v>12</v>
@@ -5439,7 +5449,7 @@
         <v>18</v>
       </c>
       <c r="H147" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I147" t="s">
         <v>20</v>
@@ -5456,7 +5466,7 @@
         <v>10</v>
       </c>
       <c r="D148" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E148" t="s">
         <v>12</v>
@@ -5468,7 +5478,7 @@
         <v>22</v>
       </c>
       <c r="H148" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I148" t="s">
         <v>24</v>
@@ -5485,7 +5495,7 @@
         <v>10</v>
       </c>
       <c r="D149" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E149" t="s">
         <v>12</v>
@@ -5514,7 +5524,7 @@
         <v>10</v>
       </c>
       <c r="D150" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E150" t="s">
         <v>12</v>
@@ -5526,7 +5536,7 @@
         <v>14</v>
       </c>
       <c r="H150" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I150" t="s">
         <v>16</v>
@@ -5543,7 +5553,7 @@
         <v>10</v>
       </c>
       <c r="D151" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E151" t="s">
         <v>12</v>
@@ -5555,7 +5565,7 @@
         <v>18</v>
       </c>
       <c r="H151" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I151" t="s">
         <v>20</v>
@@ -5572,7 +5582,7 @@
         <v>10</v>
       </c>
       <c r="D152" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E152" t="s">
         <v>12</v>
@@ -5584,7 +5594,7 @@
         <v>22</v>
       </c>
       <c r="H152" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I152" t="s">
         <v>24</v>
@@ -5601,7 +5611,7 @@
         <v>10</v>
       </c>
       <c r="D153" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E153" t="s">
         <v>12</v>
@@ -5630,7 +5640,7 @@
         <v>10</v>
       </c>
       <c r="D154" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E154" t="s">
         <v>12</v>
@@ -5642,7 +5652,7 @@
         <v>14</v>
       </c>
       <c r="H154" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I154" t="s">
         <v>16</v>
@@ -5659,7 +5669,7 @@
         <v>10</v>
       </c>
       <c r="D155" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E155" t="s">
         <v>12</v>
@@ -5671,7 +5681,7 @@
         <v>18</v>
       </c>
       <c r="H155" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I155" t="s">
         <v>20</v>
@@ -5688,7 +5698,7 @@
         <v>10</v>
       </c>
       <c r="D156" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E156" t="s">
         <v>12</v>
@@ -5700,7 +5710,7 @@
         <v>22</v>
       </c>
       <c r="H156" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I156" t="s">
         <v>24</v>
@@ -5717,7 +5727,7 @@
         <v>10</v>
       </c>
       <c r="D157" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E157" t="s">
         <v>12</v>
@@ -5746,7 +5756,7 @@
         <v>10</v>
       </c>
       <c r="D158" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E158" t="s">
         <v>12</v>
@@ -5758,7 +5768,7 @@
         <v>14</v>
       </c>
       <c r="H158" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I158" t="s">
         <v>16</v>
@@ -5775,7 +5785,7 @@
         <v>10</v>
       </c>
       <c r="D159" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E159" t="s">
         <v>12</v>
@@ -5787,7 +5797,7 @@
         <v>18</v>
       </c>
       <c r="H159" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I159" t="s">
         <v>20</v>
@@ -5804,7 +5814,7 @@
         <v>10</v>
       </c>
       <c r="D160" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E160" t="s">
         <v>12</v>
@@ -5816,7 +5826,7 @@
         <v>22</v>
       </c>
       <c r="H160" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I160" t="s">
         <v>24</v>
@@ -5833,7 +5843,7 @@
         <v>10</v>
       </c>
       <c r="D161" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E161" t="s">
         <v>12</v>
@@ -5862,7 +5872,7 @@
         <v>10</v>
       </c>
       <c r="D162" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E162" t="s">
         <v>12</v>
@@ -5874,7 +5884,7 @@
         <v>14</v>
       </c>
       <c r="H162" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I162" t="s">
         <v>16</v>
@@ -5891,7 +5901,7 @@
         <v>10</v>
       </c>
       <c r="D163" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E163" t="s">
         <v>12</v>
@@ -5903,7 +5913,7 @@
         <v>18</v>
       </c>
       <c r="H163" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I163" t="s">
         <v>20</v>
@@ -5920,7 +5930,7 @@
         <v>10</v>
       </c>
       <c r="D164" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E164" t="s">
         <v>12</v>
@@ -5932,7 +5942,7 @@
         <v>22</v>
       </c>
       <c r="H164" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I164" t="s">
         <v>24</v>
@@ -5949,7 +5959,7 @@
         <v>10</v>
       </c>
       <c r="D165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E165" t="s">
         <v>12</v>
@@ -5978,7 +5988,7 @@
         <v>10</v>
       </c>
       <c r="D166" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E166" t="s">
         <v>12</v>
@@ -5990,7 +6000,7 @@
         <v>14</v>
       </c>
       <c r="H166" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I166" t="s">
         <v>16</v>
@@ -6007,7 +6017,7 @@
         <v>10</v>
       </c>
       <c r="D167" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E167" t="s">
         <v>12</v>
@@ -6019,7 +6029,7 @@
         <v>18</v>
       </c>
       <c r="H167" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I167" t="s">
         <v>20</v>
@@ -6036,7 +6046,7 @@
         <v>10</v>
       </c>
       <c r="D168" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E168" t="s">
         <v>12</v>
@@ -6048,7 +6058,7 @@
         <v>22</v>
       </c>
       <c r="H168" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I168" t="s">
         <v>24</v>
@@ -6065,7 +6075,7 @@
         <v>10</v>
       </c>
       <c r="D169" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E169" t="s">
         <v>12</v>
@@ -6094,7 +6104,7 @@
         <v>10</v>
       </c>
       <c r="D170" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E170" t="s">
         <v>12</v>
@@ -6106,7 +6116,7 @@
         <v>14</v>
       </c>
       <c r="H170" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I170" t="s">
         <v>16</v>
@@ -6123,7 +6133,7 @@
         <v>10</v>
       </c>
       <c r="D171" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E171" t="s">
         <v>12</v>
@@ -6135,7 +6145,7 @@
         <v>18</v>
       </c>
       <c r="H171" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I171" t="s">
         <v>20</v>
@@ -6152,7 +6162,7 @@
         <v>10</v>
       </c>
       <c r="D172" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E172" t="s">
         <v>12</v>
@@ -6164,7 +6174,7 @@
         <v>22</v>
       </c>
       <c r="H172" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I172" t="s">
         <v>24</v>
@@ -6181,7 +6191,7 @@
         <v>10</v>
       </c>
       <c r="D173" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E173" t="s">
         <v>12</v>
@@ -6193,7 +6203,7 @@
         <v>26</v>
       </c>
       <c r="H173" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I173" t="s">
         <v>28</v>
@@ -6210,7 +6220,7 @@
         <v>10</v>
       </c>
       <c r="D174" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E174" t="s">
         <v>12</v>
@@ -6222,7 +6232,7 @@
         <v>14</v>
       </c>
       <c r="H174" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I174" t="s">
         <v>16</v>
@@ -6239,7 +6249,7 @@
         <v>10</v>
       </c>
       <c r="D175" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E175" t="s">
         <v>12</v>
@@ -6251,7 +6261,7 @@
         <v>18</v>
       </c>
       <c r="H175" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I175" t="s">
         <v>20</v>
@@ -6268,7 +6278,7 @@
         <v>10</v>
       </c>
       <c r="D176" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E176" t="s">
         <v>12</v>
@@ -6280,7 +6290,7 @@
         <v>22</v>
       </c>
       <c r="H176" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I176" t="s">
         <v>24</v>
@@ -6297,7 +6307,7 @@
         <v>10</v>
       </c>
       <c r="D177" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E177" t="s">
         <v>12</v>
@@ -6309,7 +6319,7 @@
         <v>26</v>
       </c>
       <c r="H177" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I177" t="s">
         <v>28</v>
@@ -6326,7 +6336,7 @@
         <v>10</v>
       </c>
       <c r="D178" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E178" t="s">
         <v>12</v>
@@ -6338,7 +6348,7 @@
         <v>14</v>
       </c>
       <c r="H178" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I178" t="s">
         <v>16</v>
@@ -6355,7 +6365,7 @@
         <v>10</v>
       </c>
       <c r="D179" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E179" t="s">
         <v>12</v>
@@ -6367,7 +6377,7 @@
         <v>18</v>
       </c>
       <c r="H179" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I179" t="s">
         <v>20</v>
@@ -6384,7 +6394,7 @@
         <v>10</v>
       </c>
       <c r="D180" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E180" t="s">
         <v>12</v>
@@ -6396,7 +6406,7 @@
         <v>22</v>
       </c>
       <c r="H180" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I180" t="s">
         <v>24</v>
@@ -6413,7 +6423,7 @@
         <v>10</v>
       </c>
       <c r="D181" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E181" t="s">
         <v>12</v>
@@ -6442,7 +6452,7 @@
         <v>10</v>
       </c>
       <c r="D182" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E182" t="s">
         <v>12</v>
@@ -6454,7 +6464,7 @@
         <v>14</v>
       </c>
       <c r="H182" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I182" t="s">
         <v>16</v>
@@ -6471,7 +6481,7 @@
         <v>10</v>
       </c>
       <c r="D183" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E183" t="s">
         <v>12</v>
@@ -6483,7 +6493,7 @@
         <v>18</v>
       </c>
       <c r="H183" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I183" t="s">
         <v>20</v>
@@ -6500,7 +6510,7 @@
         <v>10</v>
       </c>
       <c r="D184" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E184" t="s">
         <v>12</v>
@@ -6512,7 +6522,7 @@
         <v>22</v>
       </c>
       <c r="H184" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I184" t="s">
         <v>24</v>
@@ -6529,7 +6539,7 @@
         <v>10</v>
       </c>
       <c r="D185" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E185" t="s">
         <v>12</v>
@@ -6541,7 +6551,7 @@
         <v>26</v>
       </c>
       <c r="H185" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I185" t="s">
         <v>28</v>
@@ -6558,7 +6568,7 @@
         <v>10</v>
       </c>
       <c r="D186" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E186" t="s">
         <v>12</v>
@@ -6570,7 +6580,7 @@
         <v>14</v>
       </c>
       <c r="H186" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I186" t="s">
         <v>16</v>
@@ -6587,7 +6597,7 @@
         <v>10</v>
       </c>
       <c r="D187" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E187" t="s">
         <v>12</v>
@@ -6599,7 +6609,7 @@
         <v>18</v>
       </c>
       <c r="H187" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I187" t="s">
         <v>20</v>
@@ -6616,7 +6626,7 @@
         <v>10</v>
       </c>
       <c r="D188" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E188" t="s">
         <v>12</v>
@@ -6628,7 +6638,7 @@
         <v>22</v>
       </c>
       <c r="H188" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I188" t="s">
         <v>24</v>
@@ -6645,7 +6655,7 @@
         <v>10</v>
       </c>
       <c r="D189" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E189" t="s">
         <v>12</v>
@@ -6674,7 +6684,7 @@
         <v>10</v>
       </c>
       <c r="D190" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E190" t="s">
         <v>12</v>
@@ -6686,7 +6696,7 @@
         <v>14</v>
       </c>
       <c r="H190" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I190" t="s">
         <v>16</v>
@@ -6703,7 +6713,7 @@
         <v>10</v>
       </c>
       <c r="D191" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E191" t="s">
         <v>12</v>
@@ -6715,7 +6725,7 @@
         <v>18</v>
       </c>
       <c r="H191" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I191" t="s">
         <v>20</v>
@@ -6732,7 +6742,7 @@
         <v>10</v>
       </c>
       <c r="D192" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E192" t="s">
         <v>12</v>
@@ -6744,7 +6754,7 @@
         <v>22</v>
       </c>
       <c r="H192" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I192" t="s">
         <v>24</v>
@@ -6761,7 +6771,7 @@
         <v>10</v>
       </c>
       <c r="D193" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E193" t="s">
         <v>12</v>
@@ -6773,7 +6783,7 @@
         <v>26</v>
       </c>
       <c r="H193" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I193" t="s">
         <v>28</v>
@@ -6790,7 +6800,7 @@
         <v>10</v>
       </c>
       <c r="D194" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E194" t="s">
         <v>12</v>
@@ -6802,7 +6812,7 @@
         <v>14</v>
       </c>
       <c r="H194" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I194" t="s">
         <v>16</v>
@@ -6819,7 +6829,7 @@
         <v>10</v>
       </c>
       <c r="D195" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E195" t="s">
         <v>12</v>
@@ -6831,7 +6841,7 @@
         <v>18</v>
       </c>
       <c r="H195" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I195" t="s">
         <v>20</v>
@@ -6848,7 +6858,7 @@
         <v>10</v>
       </c>
       <c r="D196" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E196" t="s">
         <v>12</v>
@@ -6860,7 +6870,7 @@
         <v>22</v>
       </c>
       <c r="H196" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I196" t="s">
         <v>24</v>
@@ -6877,7 +6887,7 @@
         <v>10</v>
       </c>
       <c r="D197" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E197" t="s">
         <v>12</v>
@@ -6906,7 +6916,7 @@
         <v>10</v>
       </c>
       <c r="D198" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E198" t="s">
         <v>12</v>
@@ -6918,7 +6928,7 @@
         <v>14</v>
       </c>
       <c r="H198" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I198" t="s">
         <v>16</v>
@@ -6935,7 +6945,7 @@
         <v>10</v>
       </c>
       <c r="D199" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E199" t="s">
         <v>12</v>
@@ -6947,7 +6957,7 @@
         <v>18</v>
       </c>
       <c r="H199" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I199" t="s">
         <v>20</v>
@@ -6964,7 +6974,7 @@
         <v>10</v>
       </c>
       <c r="D200" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E200" t="s">
         <v>12</v>
@@ -6976,7 +6986,7 @@
         <v>22</v>
       </c>
       <c r="H200" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I200" t="s">
         <v>24</v>
@@ -6993,7 +7003,7 @@
         <v>10</v>
       </c>
       <c r="D201" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E201" t="s">
         <v>12</v>
@@ -7022,7 +7032,7 @@
         <v>10</v>
       </c>
       <c r="D202" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E202" t="s">
         <v>12</v>
@@ -7034,7 +7044,7 @@
         <v>14</v>
       </c>
       <c r="H202" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I202" t="s">
         <v>16</v>
@@ -7051,7 +7061,7 @@
         <v>10</v>
       </c>
       <c r="D203" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E203" t="s">
         <v>12</v>
@@ -7063,7 +7073,7 @@
         <v>18</v>
       </c>
       <c r="H203" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I203" t="s">
         <v>20</v>
@@ -7080,7 +7090,7 @@
         <v>10</v>
       </c>
       <c r="D204" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E204" t="s">
         <v>12</v>
@@ -7092,7 +7102,7 @@
         <v>22</v>
       </c>
       <c r="H204" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I204" t="s">
         <v>24</v>
@@ -7109,7 +7119,7 @@
         <v>10</v>
       </c>
       <c r="D205" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E205" t="s">
         <v>12</v>
@@ -7138,7 +7148,7 @@
         <v>10</v>
       </c>
       <c r="D206" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E206" t="s">
         <v>12</v>
@@ -7150,7 +7160,7 @@
         <v>14</v>
       </c>
       <c r="H206" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I206" t="s">
         <v>16</v>
@@ -7167,7 +7177,7 @@
         <v>10</v>
       </c>
       <c r="D207" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E207" t="s">
         <v>12</v>
@@ -7179,7 +7189,7 @@
         <v>18</v>
       </c>
       <c r="H207" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I207" t="s">
         <v>20</v>
@@ -7196,7 +7206,7 @@
         <v>10</v>
       </c>
       <c r="D208" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E208" t="s">
         <v>12</v>
@@ -7208,7 +7218,7 @@
         <v>22</v>
       </c>
       <c r="H208" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I208" t="s">
         <v>24</v>
@@ -7225,7 +7235,7 @@
         <v>10</v>
       </c>
       <c r="D209" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E209" t="s">
         <v>12</v>
@@ -7254,7 +7264,7 @@
         <v>10</v>
       </c>
       <c r="D210" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E210" t="s">
         <v>12</v>
@@ -7266,7 +7276,7 @@
         <v>14</v>
       </c>
       <c r="H210" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I210" t="s">
         <v>16</v>
@@ -7283,7 +7293,7 @@
         <v>10</v>
       </c>
       <c r="D211" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E211" t="s">
         <v>12</v>
@@ -7295,7 +7305,7 @@
         <v>18</v>
       </c>
       <c r="H211" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I211" t="s">
         <v>20</v>
@@ -7312,7 +7322,7 @@
         <v>10</v>
       </c>
       <c r="D212" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E212" t="s">
         <v>12</v>
@@ -7324,7 +7334,7 @@
         <v>22</v>
       </c>
       <c r="H212" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I212" t="s">
         <v>24</v>
@@ -7341,7 +7351,7 @@
         <v>10</v>
       </c>
       <c r="D213" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E213" t="s">
         <v>12</v>
@@ -7370,7 +7380,7 @@
         <v>10</v>
       </c>
       <c r="D214" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E214" t="s">
         <v>12</v>
@@ -7382,7 +7392,7 @@
         <v>14</v>
       </c>
       <c r="H214" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I214" t="s">
         <v>16</v>
@@ -7399,7 +7409,7 @@
         <v>10</v>
       </c>
       <c r="D215" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E215" t="s">
         <v>12</v>
@@ -7411,7 +7421,7 @@
         <v>18</v>
       </c>
       <c r="H215" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I215" t="s">
         <v>20</v>
@@ -7428,7 +7438,7 @@
         <v>10</v>
       </c>
       <c r="D216" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E216" t="s">
         <v>12</v>
@@ -7440,7 +7450,7 @@
         <v>22</v>
       </c>
       <c r="H216" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I216" t="s">
         <v>24</v>
@@ -7457,7 +7467,7 @@
         <v>10</v>
       </c>
       <c r="D217" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E217" t="s">
         <v>12</v>
@@ -7469,7 +7479,7 @@
         <v>26</v>
       </c>
       <c r="H217" t="s">
-        <v>221</v>
+        <v>124</v>
       </c>
       <c r="I217" t="s">
         <v>28</v>
@@ -7701,7 +7711,7 @@
         <v>26</v>
       </c>
       <c r="H225" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="I225" t="s">
         <v>28</v>
@@ -8629,7 +8639,7 @@
         <v>26</v>
       </c>
       <c r="H257" t="s">
-        <v>264</v>
+        <v>53</v>
       </c>
       <c r="I257" t="s">
         <v>28</v>
@@ -8646,7 +8656,7 @@
         <v>10</v>
       </c>
       <c r="D258" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E258" t="s">
         <v>12</v>
@@ -8658,7 +8668,7 @@
         <v>14</v>
       </c>
       <c r="H258" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I258" t="s">
         <v>16</v>
@@ -8675,7 +8685,7 @@
         <v>10</v>
       </c>
       <c r="D259" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E259" t="s">
         <v>12</v>
@@ -8687,7 +8697,7 @@
         <v>18</v>
       </c>
       <c r="H259" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I259" t="s">
         <v>20</v>
@@ -8704,7 +8714,7 @@
         <v>10</v>
       </c>
       <c r="D260" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E260" t="s">
         <v>12</v>
@@ -8716,7 +8726,7 @@
         <v>22</v>
       </c>
       <c r="H260" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I260" t="s">
         <v>24</v>
@@ -8733,7 +8743,7 @@
         <v>10</v>
       </c>
       <c r="D261" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E261" t="s">
         <v>12</v>
@@ -8762,7 +8772,7 @@
         <v>10</v>
       </c>
       <c r="D262" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E262" t="s">
         <v>12</v>
@@ -8774,7 +8784,7 @@
         <v>14</v>
       </c>
       <c r="H262" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I262" t="s">
         <v>16</v>
@@ -8791,7 +8801,7 @@
         <v>10</v>
       </c>
       <c r="D263" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E263" t="s">
         <v>12</v>
@@ -8803,7 +8813,7 @@
         <v>18</v>
       </c>
       <c r="H263" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I263" t="s">
         <v>20</v>
@@ -8820,7 +8830,7 @@
         <v>10</v>
       </c>
       <c r="D264" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E264" t="s">
         <v>12</v>
@@ -8832,7 +8842,7 @@
         <v>22</v>
       </c>
       <c r="H264" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I264" t="s">
         <v>24</v>
@@ -8849,7 +8859,7 @@
         <v>10</v>
       </c>
       <c r="D265" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E265" t="s">
         <v>12</v>
@@ -8878,7 +8888,7 @@
         <v>10</v>
       </c>
       <c r="D266" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E266" t="s">
         <v>12</v>
@@ -8890,7 +8900,7 @@
         <v>14</v>
       </c>
       <c r="H266" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I266" t="s">
         <v>16</v>
@@ -8907,7 +8917,7 @@
         <v>10</v>
       </c>
       <c r="D267" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E267" t="s">
         <v>12</v>
@@ -8919,7 +8929,7 @@
         <v>18</v>
       </c>
       <c r="H267" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I267" t="s">
         <v>20</v>
@@ -8936,7 +8946,7 @@
         <v>10</v>
       </c>
       <c r="D268" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E268" t="s">
         <v>12</v>
@@ -8948,7 +8958,7 @@
         <v>22</v>
       </c>
       <c r="H268" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I268" t="s">
         <v>24</v>
@@ -8965,7 +8975,7 @@
         <v>10</v>
       </c>
       <c r="D269" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E269" t="s">
         <v>12</v>
@@ -8977,7 +8987,7 @@
         <v>26</v>
       </c>
       <c r="H269" t="s">
-        <v>93</v>
+        <v>274</v>
       </c>
       <c r="I269" t="s">
         <v>28</v>
@@ -9093,7 +9103,7 @@
         <v>26</v>
       </c>
       <c r="H273" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I273" t="s">
         <v>28</v>
@@ -9208,7 +9218,9 @@
       <c r="G277" t="s">
         <v>26</v>
       </c>
-      <c r="H277"/>
+      <c r="H277" t="s">
+        <v>72</v>
+      </c>
       <c r="I277" t="s">
         <v>28</v>
       </c>

</xml_diff>